<commit_message>
new data, outlier detection
</commit_message>
<xml_diff>
--- a/Data/conductivity_field.xlsx
+++ b/Data/conductivity_field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177D571B-E0FC-4406-BC14-140C06FFFDAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A9E56-E920-4F19-BA79-8681E89DA66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31605" yWindow="1140" windowWidth="17280" windowHeight="8970" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loggers" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
     <t>datetime</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>low battery</t>
+  </si>
+  <si>
+    <t>MO- surface</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +497,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -655,7 +664,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -671,7 +680,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -691,6 +699,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1048,9 +1059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E111E348-178D-4A81-8338-72F6E909D9F1}">
   <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,9 +1144,12 @@
       <c r="D2" s="7">
         <v>43963.53125</v>
       </c>
+      <c r="E2" s="5">
+        <v>44141.5</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="20">
         <v>20758345</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1149,8 +1163,16 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4"/>
+      <c r="A4" s="22">
+        <v>20758346</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="D4" s="7"/>
+      <c r="E4" s="5">
+        <v>44141.5</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
@@ -1162,22 +1184,22 @@
       <c r="C5" s="3">
         <v>43832.604166666664</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>43845.5625</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>43851.697916666664</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>43865.677083333336</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>43865.6875</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>43906.4375</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>43906.458333333336</v>
       </c>
       <c r="J5" s="3">
@@ -1220,7 +1242,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="21">
         <v>20758346</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1243,16 +1265,16 @@
       <c r="C8" s="3">
         <v>43818.5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>43865.645833333336</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>43865.666666666664</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>43906.458333333336</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>43906.4375</v>
       </c>
       <c r="H8" s="3">
@@ -1290,16 +1312,16 @@
       <c r="C9" s="3">
         <v>43818.5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>43906.479166666664</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>43906.458333333336</v>
       </c>
       <c r="H9" s="3">
@@ -1328,20 +1350,20 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="O10" s="8">
         <v>44134.541666666664</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>20378151</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1350,16 +1372,16 @@
       <c r="C11" s="3">
         <v>43818</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>43906.416666666664</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>43906.395833333336</v>
       </c>
       <c r="H11" s="3">
@@ -1377,7 +1399,7 @@
       <c r="N11" s="8">
         <v>44126.520833333336</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1391,16 +1413,16 @@
       <c r="C12" s="3">
         <v>43818</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>43865.645833333336</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>43865.666666666664</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>43906.458333333336</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>43906.4375</v>
       </c>
       <c r="H12" s="3">
@@ -1438,16 +1460,16 @@
       <c r="C13" s="3">
         <v>43818</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>43865.625</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>43865.645833333336</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>43906.416666666664</v>
       </c>
       <c r="H13" s="3">
@@ -1485,16 +1507,16 @@
       <c r="C14" s="3">
         <v>43818</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>43865.604166666664</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>43865.625</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>43906.416666666664</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>43906.395833333336</v>
       </c>
       <c r="H14" s="3">
@@ -1526,16 +1548,16 @@
       <c r="C15" s="3">
         <v>43818</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>43906.375</v>
       </c>
       <c r="H15" s="3">
@@ -1558,7 +1580,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>20758345</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1567,12 +1589,12 @@
       <c r="C16" s="3">
         <v>43999.666666666664</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
@@ -1592,7 +1614,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>20484276</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1604,7 +1626,7 @@
       <c r="D21" s="7">
         <v>43906.364583333336</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>43906.375</v>
       </c>
       <c r="F21" s="3">
@@ -1641,7 +1663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1906,7 +1928,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+      <c r="A24" s="19">
         <v>44082.463194444441</v>
       </c>
       <c r="B24">
@@ -2047,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588D9C27-B403-4DE5-8B68-B5C4B22BE996}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2185,6 +2207,90 @@
       </c>
       <c r="D9">
         <v>24.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44141.43472222222</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>392.5</v>
+      </c>
+      <c r="D10">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44141.448611111111</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>393.8</v>
+      </c>
+      <c r="D11">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44141.446527777778</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>390.3</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44141.443055555559</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>395.2</v>
+      </c>
+      <c r="D13">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44141.439583333333</v>
+      </c>
+      <c r="B14" s="2">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>392.5</v>
+      </c>
+      <c r="D14">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44141.4375</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>392.8</v>
+      </c>
+      <c r="D15">
+        <v>8.8000000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of trouble, but working through it slowly.
</commit_message>
<xml_diff>
--- a/Data/conductivity_field.xlsx
+++ b/Data/conductivity_field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A9E56-E920-4F19-BA79-8681E89DA66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2A36B0-B8D4-494C-96F5-EA9E44594CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30630" yWindow="1890" windowWidth="17280" windowHeight="8970" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loggers" sheetId="12" r:id="rId1"/>
@@ -664,7 +664,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -693,8 +693,6 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="165" fontId="14" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1059,9 +1057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E111E348-178D-4A81-8338-72F6E909D9F1}">
   <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1147,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>20758345</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1163,7 +1161,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="20">
         <v>20758346</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1242,7 +1240,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="19">
         <v>20758346</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1350,7 +1348,9 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
+      <c r="A10">
+        <v>20882401</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1589,12 +1589,14 @@
       <c r="C16" s="3">
         <v>43999.666666666664</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17">
+        <v>20882406</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
@@ -1661,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1928,7 +1930,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="A24" s="17">
         <v>44082.463194444441</v>
       </c>
       <c r="B24">
@@ -1969,6 +1971,17 @@
       </c>
       <c r="C27">
         <v>5.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44152.589583333334</v>
+      </c>
+      <c r="B28">
+        <v>230.2</v>
+      </c>
+      <c r="C28">
+        <v>4.8</v>
       </c>
     </row>
   </sheetData>
@@ -2301,10 +2314,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7E974B-BCA0-45B0-95FE-63AB262733E9}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2435,6 +2448,17 @@
         <v>4.3</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44152.423611111109</v>
+      </c>
+      <c r="B12">
+        <v>480.5</v>
+      </c>
+      <c r="C12">
+        <v>2.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2442,10 +2466,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2741,6 +2765,17 @@
         <v>8.5</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44152.438888888886</v>
+      </c>
+      <c r="B27">
+        <v>347.4</v>
+      </c>
+      <c r="C27">
+        <v>4.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2752,7 +2787,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3093,6 +3128,15 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44152.459027777775</v>
+      </c>
+      <c r="B26">
+        <v>682.5</v>
+      </c>
+      <c r="C26">
+        <v>3.9</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -3130,10 +3174,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3407,6 +3451,17 @@
         <v>7.5</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44152.475694444445</v>
+      </c>
+      <c r="B25">
+        <v>343.1</v>
+      </c>
+      <c r="C25">
+        <v>5.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3414,10 +3469,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3691,6 +3746,17 @@
         <v>3.4</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44152.529166666667</v>
+      </c>
+      <c r="B25">
+        <v>378</v>
+      </c>
+      <c r="C25">
+        <v>2.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3698,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3986,6 +4052,17 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44152.541666666664</v>
+      </c>
+      <c r="B26">
+        <v>433</v>
+      </c>
+      <c r="C26">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3993,10 +4070,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4281,6 +4358,17 @@
         <v>4.8</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44152.554861111108</v>
+      </c>
+      <c r="B26">
+        <v>510</v>
+      </c>
+      <c r="C26">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4288,10 +4376,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,6 +4675,17 @@
         <v>5.2</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44152.576388888891</v>
+      </c>
+      <c r="B27">
+        <v>517.4</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chloride loads and q-c plots
</commit_message>
<xml_diff>
--- a/Data/conductivity_field.xlsx
+++ b/Data/conductivity_field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55ECFE3-0B06-48B2-93EF-35956FB52A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939EB2AF-96E0-4962-BBA6-489BDC4A81EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loggers" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
   <si>
     <t>datetime</t>
   </si>
@@ -1744,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2107,6 +2107,11 @@
       </c>
       <c r="C32">
         <v>3.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>44201.566666666666</v>
       </c>
     </row>
   </sheetData>
@@ -2523,10 +2528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7E974B-BCA0-45B0-95FE-63AB262733E9}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2712,6 +2717,17 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44201.415972222225</v>
+      </c>
+      <c r="B17">
+        <v>520.1</v>
+      </c>
+      <c r="C17">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2719,10 +2735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3073,6 +3089,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44201.432638888888</v>
+      </c>
+      <c r="B32">
+        <v>315.89999999999998</v>
+      </c>
+      <c r="C32">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3083,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,6 +3521,15 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44201.45</v>
+      </c>
+      <c r="B31">
+        <v>714</v>
+      </c>
+      <c r="C31">
+        <v>2.1</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
@@ -3507,10 +3543,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3546,12 +3582,6 @@
       <c r="A3" s="1">
         <v>43830.57708333333</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -3837,6 +3867,17 @@
       </c>
       <c r="C29">
         <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44201.464583333334</v>
+      </c>
+      <c r="B30">
+        <v>309.8</v>
+      </c>
+      <c r="C30">
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>
@@ -3846,345 +3887,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43818.638888888891</v>
-      </c>
-      <c r="B2">
-        <v>452.2</v>
-      </c>
-      <c r="C2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43830.6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>43836.447222222225</v>
-      </c>
-      <c r="B4">
-        <v>425.2</v>
-      </c>
-      <c r="C4">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>43844.600694444445</v>
-      </c>
-      <c r="B5">
-        <v>437.8</v>
-      </c>
-      <c r="C5">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>43851.635416666664</v>
-      </c>
-      <c r="B6">
-        <v>453.4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43858.625</v>
-      </c>
-      <c r="B7">
-        <v>457.6</v>
-      </c>
-      <c r="C7">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>43865.629166666666</v>
-      </c>
-      <c r="B8">
-        <v>432.1</v>
-      </c>
-      <c r="C8">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>43872.621527777781</v>
-      </c>
-      <c r="B9">
-        <v>512.36</v>
-      </c>
-      <c r="C9">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>43879.131249999999</v>
-      </c>
-      <c r="B10">
-        <v>442.3</v>
-      </c>
-      <c r="C10">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>43886.615972222222</v>
-      </c>
-      <c r="B11">
-        <v>451.3</v>
-      </c>
-      <c r="C11">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>43893.629166666666</v>
-      </c>
-      <c r="B12">
-        <v>476.7</v>
-      </c>
-      <c r="C12">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>43900.574305555558</v>
-      </c>
-      <c r="B13">
-        <v>353.7</v>
-      </c>
-      <c r="C13">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>43906.40625</v>
-      </c>
-      <c r="B14">
-        <v>409.7</v>
-      </c>
-      <c r="C14">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>43999.487500000003</v>
-      </c>
-      <c r="B15">
-        <v>487.5</v>
-      </c>
-      <c r="C15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>44012.429861111108</v>
-      </c>
-      <c r="B16">
-        <v>682.5</v>
-      </c>
-      <c r="C16">
-        <v>27.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>44026.414583333331</v>
-      </c>
-      <c r="B17">
-        <v>493.5</v>
-      </c>
-      <c r="C17">
-        <v>26.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>44040.37222222222</v>
-      </c>
-      <c r="B18">
-        <v>687.5</v>
-      </c>
-      <c r="C18">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>44054.408333333333</v>
-      </c>
-      <c r="B19">
-        <v>687.1</v>
-      </c>
-      <c r="C19">
-        <v>24.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>44069.425000000003</v>
-      </c>
-      <c r="B20">
-        <v>724.4</v>
-      </c>
-      <c r="C20">
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>44082.409722222219</v>
-      </c>
-      <c r="B21">
-        <v>557.4</v>
-      </c>
-      <c r="C21">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>44096.418749999997</v>
-      </c>
-      <c r="B22">
-        <v>571.1</v>
-      </c>
-      <c r="C22">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>44110.392361111109</v>
-      </c>
-      <c r="B23">
-        <v>553.5</v>
-      </c>
-      <c r="C23">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>44134.345138888886</v>
-      </c>
-      <c r="B24">
-        <v>344.1</v>
-      </c>
-      <c r="C24">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>44152.529166666667</v>
-      </c>
-      <c r="B25">
-        <v>378</v>
-      </c>
-      <c r="C25">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>44159.513194444444</v>
-      </c>
-      <c r="B26">
-        <v>441.4</v>
-      </c>
-      <c r="C26">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>44169.482638888891</v>
-      </c>
-      <c r="B27">
-        <v>439</v>
-      </c>
-      <c r="C27">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>44180.623611111114</v>
-      </c>
-      <c r="B28">
-        <v>445.7</v>
-      </c>
-      <c r="C28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>44194.457638888889</v>
-      </c>
-      <c r="B29">
-        <v>471.8</v>
-      </c>
-      <c r="C29">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -4211,32 +3913,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>43818.631249999999</v>
+        <v>43818.638888888891</v>
       </c>
       <c r="B2">
-        <v>450.3</v>
+        <v>452.2</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>43830.619444444441</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+        <v>43830.6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>43836.461111111108</v>
+        <v>43836.447222222225</v>
       </c>
       <c r="B4">
-        <v>431.8</v>
+        <v>425.2</v>
       </c>
       <c r="C4">
         <v>1.2</v>
@@ -4244,54 +3940,54 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>43844.62777777778</v>
+        <v>43844.600694444445</v>
       </c>
       <c r="B5">
-        <v>484.4</v>
+        <v>437.8</v>
       </c>
       <c r="C5">
-        <v>3.7</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>43851.649305555555</v>
+        <v>43851.635416666664</v>
       </c>
       <c r="B6">
-        <v>240.7</v>
+        <v>453.4</v>
       </c>
       <c r="C6">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>43858.634027777778</v>
+        <v>43858.625</v>
       </c>
       <c r="B7">
-        <v>480.5</v>
+        <v>457.6</v>
       </c>
       <c r="C7">
-        <v>2.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>43865.643055555556</v>
+        <v>43865.629166666666</v>
       </c>
       <c r="B8">
-        <v>471</v>
+        <v>432.1</v>
       </c>
       <c r="C8">
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>43872.629861111112</v>
+        <v>43872.621527777781</v>
       </c>
       <c r="B9">
-        <v>489.8</v>
+        <v>512.36</v>
       </c>
       <c r="C9">
         <v>2.2000000000000002</v>
@@ -4299,219 +3995,219 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>43879.640277777777</v>
+        <v>43879.131249999999</v>
       </c>
       <c r="B10">
-        <v>525.5</v>
+        <v>442.3</v>
       </c>
       <c r="C10">
-        <v>3.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>43886.625</v>
+        <v>43886.615972222222</v>
       </c>
       <c r="B11">
-        <v>520.79999999999995</v>
+        <v>451.3</v>
       </c>
       <c r="C11">
-        <v>4.0999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>43893.638888888891</v>
+        <v>43893.629166666666</v>
       </c>
       <c r="B12">
-        <v>415.7</v>
+        <v>476.7</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>43900.582638888889</v>
+        <v>43900.574305555558</v>
       </c>
       <c r="B13">
-        <v>374.8</v>
+        <v>353.7</v>
       </c>
       <c r="C13">
-        <v>5.6</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>43906.416666666664</v>
+        <v>43906.40625</v>
       </c>
       <c r="B14">
-        <v>452.8</v>
+        <v>409.7</v>
       </c>
       <c r="C14">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>43999.46875</v>
+        <v>43999.487500000003</v>
       </c>
       <c r="B15">
-        <v>708.6</v>
+        <v>487.5</v>
       </c>
       <c r="C15">
-        <v>22.4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44012.448611111111</v>
+        <v>44012.429861111108</v>
       </c>
       <c r="B16">
-        <v>683.1</v>
+        <v>682.5</v>
       </c>
       <c r="C16">
-        <v>23</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44026.395833333336</v>
+        <v>44026.414583333331</v>
       </c>
       <c r="B17">
-        <v>508.5</v>
+        <v>493.5</v>
       </c>
       <c r="C17">
-        <v>23.2</v>
+        <v>26.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44033.688194444447</v>
+        <v>44040.37222222222</v>
       </c>
       <c r="B18">
-        <v>657.5</v>
+        <v>687.5</v>
       </c>
       <c r="C18">
-        <v>22.9</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44040.383333333331</v>
+        <v>44054.408333333333</v>
       </c>
       <c r="B19">
-        <v>701.5</v>
+        <v>687.1</v>
       </c>
       <c r="C19">
-        <v>22.3</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44054.422222222223</v>
+        <v>44069.425000000003</v>
       </c>
       <c r="B20">
-        <v>716.3</v>
+        <v>724.4</v>
       </c>
       <c r="C20">
-        <v>20.7</v>
+        <v>26.8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>44069.443055555559</v>
+        <v>44082.409722222219</v>
       </c>
       <c r="B21">
-        <v>818.4</v>
+        <v>557.4</v>
       </c>
       <c r="C21">
-        <v>22.9</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>44082.429166666669</v>
+        <v>44096.418749999997</v>
       </c>
       <c r="B22">
-        <v>660.2</v>
+        <v>571.1</v>
       </c>
       <c r="C22">
-        <v>14.4</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>44096.436111111114</v>
+        <v>44110.392361111109</v>
       </c>
       <c r="B23">
-        <v>674</v>
+        <v>553.5</v>
       </c>
       <c r="C23">
-        <v>15.5</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>44110.406944444447</v>
+        <v>44134.345138888886</v>
       </c>
       <c r="B24">
-        <v>651.79999999999995</v>
+        <v>344.1</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>44134.35833333333</v>
+        <v>44152.529166666667</v>
       </c>
       <c r="B25">
-        <v>440.1</v>
+        <v>378</v>
       </c>
       <c r="C25">
-        <v>4.0999999999999996</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>44152.541666666664</v>
+        <v>44159.513194444444</v>
       </c>
       <c r="B26">
-        <v>433</v>
+        <v>441.4</v>
       </c>
       <c r="C26">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>44159.520833333336</v>
+        <v>44169.482638888891</v>
       </c>
       <c r="B27">
-        <v>469.8</v>
+        <v>439</v>
       </c>
       <c r="C27">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>44169.536805555559</v>
+        <v>44180.623611111114</v>
       </c>
       <c r="B28">
-        <v>498.3</v>
+        <v>445.7</v>
       </c>
       <c r="C28">
-        <v>3.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>44180.638194444444</v>
+        <v>44194.457638888889</v>
       </c>
       <c r="B29">
-        <v>457.5</v>
+        <v>471.8</v>
       </c>
       <c r="C29">
         <v>0.1</v>
@@ -4519,13 +4215,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>44194.466666666667</v>
+        <v>44201.527777777781</v>
       </c>
       <c r="B30">
-        <v>474.1</v>
+        <v>427.8</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>
@@ -4533,361 +4229,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C30"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43818.62222222222</v>
-      </c>
-      <c r="B2">
-        <v>472</v>
-      </c>
-      <c r="C2">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43830.627083333333</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>43836.46875</v>
-      </c>
-      <c r="B4">
-        <v>463.7</v>
-      </c>
-      <c r="C4">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>43844.637499999997</v>
-      </c>
-      <c r="B5">
-        <v>493.2</v>
-      </c>
-      <c r="C5">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>43851.659722222219</v>
-      </c>
-      <c r="B6">
-        <v>435.5</v>
-      </c>
-      <c r="C6">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43858.642361111109</v>
-      </c>
-      <c r="B7">
-        <v>490.2</v>
-      </c>
-      <c r="C7">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>43865.654166666667</v>
-      </c>
-      <c r="B8">
-        <v>506</v>
-      </c>
-      <c r="C8">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>43872.634722222225</v>
-      </c>
-      <c r="B9">
-        <v>494.6</v>
-      </c>
-      <c r="C9">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>43879.645833333336</v>
-      </c>
-      <c r="B10">
-        <v>574.4</v>
-      </c>
-      <c r="C10">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>43886.631249999999</v>
-      </c>
-      <c r="B11">
-        <v>783.8</v>
-      </c>
-      <c r="C11">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>43893.652777777781</v>
-      </c>
-      <c r="B12">
-        <v>389.7</v>
-      </c>
-      <c r="C12">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>43900.59097222222</v>
-      </c>
-      <c r="B13">
-        <v>432.3</v>
-      </c>
-      <c r="C13">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>43906.427083333336</v>
-      </c>
-      <c r="B14">
-        <v>491.8</v>
-      </c>
-      <c r="C14">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>43999.447916666664</v>
-      </c>
-      <c r="B15">
-        <v>716.6</v>
-      </c>
-      <c r="C15">
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>44012.457638888889</v>
-      </c>
-      <c r="B16">
-        <v>588.1</v>
-      </c>
-      <c r="C16">
-        <v>21.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>44026.385416666664</v>
-      </c>
-      <c r="B17">
-        <v>722</v>
-      </c>
-      <c r="C17">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>44033.677083333336</v>
-      </c>
-      <c r="B18">
-        <v>758.7</v>
-      </c>
-      <c r="C18">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>44040.393055555556</v>
-      </c>
-      <c r="B19">
-        <v>687.5</v>
-      </c>
-      <c r="C19">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>44054.429861111108</v>
-      </c>
-      <c r="B20">
-        <v>719.9</v>
-      </c>
-      <c r="C20">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>44069.454861111109</v>
-      </c>
-      <c r="B21">
-        <v>766.8</v>
-      </c>
-      <c r="C21">
-        <v>20.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>44082.439583333333</v>
-      </c>
-      <c r="B22">
-        <v>657.8</v>
-      </c>
-      <c r="C22">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>44096.444444444445</v>
-      </c>
-      <c r="B23">
-        <v>679.2</v>
-      </c>
-      <c r="C23">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>44110.415277777778</v>
-      </c>
-      <c r="B24">
-        <v>621.70000000000005</v>
-      </c>
-      <c r="C24">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>44134.368055555555</v>
-      </c>
-      <c r="B25">
-        <v>514.9</v>
-      </c>
-      <c r="C25">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>44152.554861111108</v>
-      </c>
-      <c r="B26">
-        <v>510</v>
-      </c>
-      <c r="C26">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>44159.52847222222</v>
-      </c>
-      <c r="B27">
-        <v>483.3</v>
-      </c>
-      <c r="C27">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>44169.541666666664</v>
-      </c>
-      <c r="B28">
-        <v>507.9</v>
-      </c>
-      <c r="C28">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>44180.649305555555</v>
-      </c>
-      <c r="B29">
-        <v>449.3</v>
-      </c>
-      <c r="C29">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>44194.474305555559</v>
-      </c>
-      <c r="B30">
-        <v>456</v>
-      </c>
-      <c r="C30">
-        <v>0.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -4911,6 +4257,728 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <v>43818.631249999999</v>
+      </c>
+      <c r="B2">
+        <v>450.3</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43830.619444444441</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43836.461111111108</v>
+      </c>
+      <c r="B4">
+        <v>431.8</v>
+      </c>
+      <c r="C4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43844.62777777778</v>
+      </c>
+      <c r="B5">
+        <v>484.4</v>
+      </c>
+      <c r="C5">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43851.649305555555</v>
+      </c>
+      <c r="B6">
+        <v>240.7</v>
+      </c>
+      <c r="C6">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43858.634027777778</v>
+      </c>
+      <c r="B7">
+        <v>480.5</v>
+      </c>
+      <c r="C7">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43865.643055555556</v>
+      </c>
+      <c r="B8">
+        <v>471</v>
+      </c>
+      <c r="C8">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43872.629861111112</v>
+      </c>
+      <c r="B9">
+        <v>489.8</v>
+      </c>
+      <c r="C9">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43879.640277777777</v>
+      </c>
+      <c r="B10">
+        <v>525.5</v>
+      </c>
+      <c r="C10">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>43886.625</v>
+      </c>
+      <c r="B11">
+        <v>520.79999999999995</v>
+      </c>
+      <c r="C11">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>43893.638888888891</v>
+      </c>
+      <c r="B12">
+        <v>415.7</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>43900.582638888889</v>
+      </c>
+      <c r="B13">
+        <v>374.8</v>
+      </c>
+      <c r="C13">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>43906.416666666664</v>
+      </c>
+      <c r="B14">
+        <v>452.8</v>
+      </c>
+      <c r="C14">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>43999.46875</v>
+      </c>
+      <c r="B15">
+        <v>708.6</v>
+      </c>
+      <c r="C15">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44012.448611111111</v>
+      </c>
+      <c r="B16">
+        <v>683.1</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44026.395833333336</v>
+      </c>
+      <c r="B17">
+        <v>508.5</v>
+      </c>
+      <c r="C17">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44033.688194444447</v>
+      </c>
+      <c r="B18">
+        <v>657.5</v>
+      </c>
+      <c r="C18">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44040.383333333331</v>
+      </c>
+      <c r="B19">
+        <v>701.5</v>
+      </c>
+      <c r="C19">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44054.422222222223</v>
+      </c>
+      <c r="B20">
+        <v>716.3</v>
+      </c>
+      <c r="C20">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44069.443055555559</v>
+      </c>
+      <c r="B21">
+        <v>818.4</v>
+      </c>
+      <c r="C21">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44082.429166666669</v>
+      </c>
+      <c r="B22">
+        <v>660.2</v>
+      </c>
+      <c r="C22">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44096.436111111114</v>
+      </c>
+      <c r="B23">
+        <v>674</v>
+      </c>
+      <c r="C23">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44110.406944444447</v>
+      </c>
+      <c r="B24">
+        <v>651.79999999999995</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44134.35833333333</v>
+      </c>
+      <c r="B25">
+        <v>440.1</v>
+      </c>
+      <c r="C25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44152.541666666664</v>
+      </c>
+      <c r="B26">
+        <v>433</v>
+      </c>
+      <c r="C26">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44159.520833333336</v>
+      </c>
+      <c r="B27">
+        <v>469.8</v>
+      </c>
+      <c r="C27">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44169.536805555559</v>
+      </c>
+      <c r="B28">
+        <v>498.3</v>
+      </c>
+      <c r="C28">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44180.638194444444</v>
+      </c>
+      <c r="B29">
+        <v>457.5</v>
+      </c>
+      <c r="C29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44194.466666666667</v>
+      </c>
+      <c r="B30">
+        <v>474.1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44201.536805555559</v>
+      </c>
+      <c r="B31">
+        <v>472</v>
+      </c>
+      <c r="C31">
+        <v>2.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43818.62222222222</v>
+      </c>
+      <c r="B2">
+        <v>472</v>
+      </c>
+      <c r="C2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43830.627083333333</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43836.46875</v>
+      </c>
+      <c r="B4">
+        <v>463.7</v>
+      </c>
+      <c r="C4">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43844.637499999997</v>
+      </c>
+      <c r="B5">
+        <v>493.2</v>
+      </c>
+      <c r="C5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43851.659722222219</v>
+      </c>
+      <c r="B6">
+        <v>435.5</v>
+      </c>
+      <c r="C6">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43858.642361111109</v>
+      </c>
+      <c r="B7">
+        <v>490.2</v>
+      </c>
+      <c r="C7">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43865.654166666667</v>
+      </c>
+      <c r="B8">
+        <v>506</v>
+      </c>
+      <c r="C8">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43872.634722222225</v>
+      </c>
+      <c r="B9">
+        <v>494.6</v>
+      </c>
+      <c r="C9">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43879.645833333336</v>
+      </c>
+      <c r="B10">
+        <v>574.4</v>
+      </c>
+      <c r="C10">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>43886.631249999999</v>
+      </c>
+      <c r="B11">
+        <v>783.8</v>
+      </c>
+      <c r="C11">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>43893.652777777781</v>
+      </c>
+      <c r="B12">
+        <v>389.7</v>
+      </c>
+      <c r="C12">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>43900.59097222222</v>
+      </c>
+      <c r="B13">
+        <v>432.3</v>
+      </c>
+      <c r="C13">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>43906.427083333336</v>
+      </c>
+      <c r="B14">
+        <v>491.8</v>
+      </c>
+      <c r="C14">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>43999.447916666664</v>
+      </c>
+      <c r="B15">
+        <v>716.6</v>
+      </c>
+      <c r="C15">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44012.457638888889</v>
+      </c>
+      <c r="B16">
+        <v>588.1</v>
+      </c>
+      <c r="C16">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44026.385416666664</v>
+      </c>
+      <c r="B17">
+        <v>722</v>
+      </c>
+      <c r="C17">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44033.677083333336</v>
+      </c>
+      <c r="B18">
+        <v>758.7</v>
+      </c>
+      <c r="C18">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44040.393055555556</v>
+      </c>
+      <c r="B19">
+        <v>687.5</v>
+      </c>
+      <c r="C19">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44054.429861111108</v>
+      </c>
+      <c r="B20">
+        <v>719.9</v>
+      </c>
+      <c r="C20">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44069.454861111109</v>
+      </c>
+      <c r="B21">
+        <v>766.8</v>
+      </c>
+      <c r="C21">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44082.439583333333</v>
+      </c>
+      <c r="B22">
+        <v>657.8</v>
+      </c>
+      <c r="C22">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44096.444444444445</v>
+      </c>
+      <c r="B23">
+        <v>679.2</v>
+      </c>
+      <c r="C23">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44110.415277777778</v>
+      </c>
+      <c r="B24">
+        <v>621.70000000000005</v>
+      </c>
+      <c r="C24">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44134.368055555555</v>
+      </c>
+      <c r="B25">
+        <v>514.9</v>
+      </c>
+      <c r="C25">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44152.554861111108</v>
+      </c>
+      <c r="B26">
+        <v>510</v>
+      </c>
+      <c r="C26">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44159.52847222222</v>
+      </c>
+      <c r="B27">
+        <v>483.3</v>
+      </c>
+      <c r="C27">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44169.541666666664</v>
+      </c>
+      <c r="B28">
+        <v>507.9</v>
+      </c>
+      <c r="C28">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44180.649305555555</v>
+      </c>
+      <c r="B29">
+        <v>449.3</v>
+      </c>
+      <c r="C29">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44194.474305555559</v>
+      </c>
+      <c r="B30">
+        <v>456</v>
+      </c>
+      <c r="C30">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44201.543055555558</v>
+      </c>
+      <c r="B31">
+        <v>476.3</v>
+      </c>
+      <c r="C31">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>43818.609722222223</v>
       </c>
       <c r="B2">
@@ -5237,6 +5305,17 @@
       </c>
       <c r="C31">
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44201.558333333334</v>
+      </c>
+      <c r="B32">
+        <v>663.2</v>
+      </c>
+      <c r="C32">
+        <v>2.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>